<commit_message>
Begin making SciAv dataset, clean up the raw meter files and change them to be summary files
Since I'm no longer using the metering data from the summary files, it is confusing to include those data so I deleted those columns in the CSV files
</commit_message>
<xml_diff>
--- a/02_meter_data/meter_sizing_graphs/uncertainty_summary.xlsx
+++ b/02_meter_data/meter_sizing_graphs/uncertainty_summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sea/PycharmProjects/CRF22_Airplanes/02_meter_data/meter_sizing_graphs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B34B906C-BAFD-7941-A389-6578C56D265B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5208644A-7BEA-4642-9C90-7A2C3A934D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="760" windowWidth="33360" windowHeight="16940" activeTab="2" xr2:uid="{BA59B2C7-F1E3-E647-91B8-3B4014987930}"/>
+    <workbookView xWindow="300" yWindow="760" windowWidth="33360" windowHeight="16940" activeTab="2" xr2:uid="{BA59B2C7-F1E3-E647-91B8-3B4014987930}"/>
   </bookViews>
   <sheets>
     <sheet name="baby_corey" sheetId="1" r:id="rId1"/>
@@ -4017,7 +4017,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:C23"/>
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>